<commit_message>
Add individual reader and fix bugs.
</commit_message>
<xml_diff>
--- a/test/helper/estrus_data/estrus_data.xlsx
+++ b/test/helper/estrus_data/estrus_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{352BBBF8-AB6F-4262-9097-A994CF1B6E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3AEE805-1871-4325-96CE-5014DF72019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基本資料" sheetId="1" r:id="rId1"/>
-    <sheet name="配種資料" sheetId="2" r:id="rId2"/>
+    <sheet name="發情資料" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="142">
   <si>
     <t>序號</t>
   </si>
@@ -419,25 +419,16 @@
     <t>1017-3</t>
   </si>
   <si>
+    <t>出生年品種耳號</t>
+  </si>
+  <si>
     <t>胎次</t>
   </si>
   <si>
-    <t>與配公豬</t>
-  </si>
-  <si>
-    <t>配種日期</t>
-  </si>
-  <si>
-    <t>週次</t>
-  </si>
-  <si>
-    <t>配種時間</t>
-  </si>
-  <si>
-    <t>配種次數</t>
-  </si>
-  <si>
-    <t>豬隻特徵</t>
+    <t>發情日期</t>
+  </si>
+  <si>
+    <t>發情時間</t>
   </si>
   <si>
     <t>21天測孕</t>
@@ -446,19 +437,22 @@
     <t>60天測孕</t>
   </si>
   <si>
-    <t>事發日期</t>
-  </si>
-  <si>
-    <t>事發狀況</t>
-  </si>
-  <si>
-    <t>生日年品種耳號胎次</t>
+    <t>問題</t>
   </si>
   <si>
     <t>隨機耳號</t>
   </si>
   <si>
     <t>隨機發情日</t>
+  </si>
+  <si>
+    <t>胎號</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>不同耳號格式</t>
@@ -864,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3233,1346 +3227,1904 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9635F25D-E9A9-4A49-B6C3-EDF6A09A71EB}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53:XFD53"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2:J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" t="s">
         <v>123</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="E1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
       <c r="G1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N2), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N2), INDEX(基本資料!$C$51:$C$101, 配種資料!N2))</f>
+        <f t="array" ref="A2">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H2), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H2), INDEX(基本資料!$C$51:$C$101, 發情資料!H2))</f>
         <v>18D1714-3</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="1" cm="1">
-        <f t="array" ref="D2">INDEX(基本資料!$E$51:$E$101, 配種資料!N2) + 配種資料!O2</f>
+      <c r="C2" s="1" cm="1">
+        <f t="array" ref="C2">INDEX(基本資料!$E$51:$E$101, 發情資料!H2) + 發情資料!I2</f>
         <v>43299</v>
       </c>
-      <c r="F2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
+      <c r="D2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>182</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="J2">
+        <f ca="1">RANDBETWEEN(1000,2000)</f>
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N3), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N3), INDEX(基本資料!$C$51:$C$101, 配種資料!N3))</f>
+        <f t="array" ref="A3">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H3), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H3), INDEX(基本資料!$C$51:$C$101, 發情資料!H3))</f>
         <v>18D1714-3</v>
       </c>
       <c r="B3">
         <f>IF(A2=A3, B2+1, 1)</f>
         <v>2</v>
       </c>
-      <c r="D3" s="1" cm="1">
-        <f t="array" ref="D3">INDEX(基本資料!$E$51:$E$101, 配種資料!N3) + 配種資料!O3</f>
+      <c r="C3" s="1" cm="1">
+        <f t="array" ref="C3">INDEX(基本資料!$E$51:$E$101, 發情資料!H3) + 發情資料!I3</f>
         <v>43485</v>
       </c>
-      <c r="F3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>368</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="J3">
+        <f t="shared" ref="J3:J59" ca="1" si="0">RANDBETWEEN(1000,2000)</f>
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="str" cm="1">
-        <f t="array" ref="A4">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N4), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N4), INDEX(基本資料!$C$51:$C$101, 配種資料!N4))</f>
+        <f t="array" ref="A4">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H4), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H4), INDEX(基本資料!$C$51:$C$101, 發情資料!H4))</f>
         <v>20L1722-15</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B51" si="0">IF(A3=A4, B3+1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" cm="1">
-        <f t="array" ref="D4">INDEX(基本資料!$E$51:$E$101, 配種資料!N4) + 配種資料!O4</f>
+        <f t="shared" ref="B4:B51" si="1">IF(A3=A4, B3+1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" cm="1">
+        <f t="array" ref="C4">INDEX(基本資料!$E$51:$E$101, 發情資料!H4) + 發情資料!I4</f>
         <v>44215</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
+      <c r="D4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
         <v>188</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="J4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="str" cm="1">
-        <f t="array" ref="A5">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N5), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N5), INDEX(基本資料!$C$51:$C$101, 配種資料!N5))</f>
+        <f t="array" ref="A5">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H5), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H5), INDEX(基本資料!$C$51:$C$101, 發情資料!H5))</f>
         <v>22L1099-11</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" cm="1">
-        <f t="array" ref="D5">INDEX(基本資料!$E$51:$E$101, 配種資料!N5) + 配種資料!O5</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" cm="1">
+        <f t="array" ref="C5">INDEX(基本資料!$E$51:$E$101, 發情資料!H5) + 發情資料!I5</f>
         <v>45025</v>
       </c>
-      <c r="F5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N5">
+      <c r="D5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="O5">
+      <c r="I5">
         <v>190</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="str" cm="1">
-        <f t="array" ref="A6">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N6), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N6), INDEX(基本資料!$C$51:$C$101, 配種資料!N6))</f>
+        <f t="array" ref="A6">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H6), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H6), INDEX(基本資料!$C$51:$C$101, 發情資料!H6))</f>
         <v>22L1099-11</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" cm="1">
-        <f t="array" ref="D6">INDEX(基本資料!$E$51:$E$101, 配種資料!N6) + 配種資料!O6</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" cm="1">
+        <f t="array" ref="C6">INDEX(基本資料!$E$51:$E$101, 發情資料!H6) + 發情資料!I6</f>
         <v>45213</v>
       </c>
-      <c r="F6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N6">
+      <c r="D6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="O6">
+      <c r="I6">
         <v>378</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="str" cm="1">
-        <f t="array" ref="A7">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N7), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N7), INDEX(基本資料!$C$51:$C$101, 配種資料!N7))</f>
+        <f t="array" ref="A7">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H7), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H7), INDEX(基本資料!$C$51:$C$101, 發情資料!H7))</f>
         <v>17L1315-10</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" cm="1">
-        <f t="array" ref="D7">INDEX(基本資料!$E$51:$E$101, 配種資料!N7) + 配種資料!O7</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" cm="1">
+        <f t="array" ref="C7">INDEX(基本資料!$E$51:$E$101, 發情資料!H7) + 發情資料!I7</f>
         <v>43077</v>
       </c>
-      <c r="F7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N7">
+      <c r="D7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7">
         <v>5</v>
       </c>
-      <c r="O7">
+      <c r="I7">
         <v>185</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="str" cm="1">
-        <f t="array" ref="A8">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N8), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N8), INDEX(基本資料!$C$51:$C$101, 配種資料!N8))</f>
+        <f t="array" ref="A8">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H8), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H8), INDEX(基本資料!$C$51:$C$101, 發情資料!H8))</f>
         <v>18D1501-2</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" cm="1">
-        <f t="array" ref="D8">INDEX(基本資料!$E$51:$E$101, 配種資料!N8) + 配種資料!O8</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" cm="1">
+        <f t="array" ref="C8">INDEX(基本資料!$E$51:$E$101, 發情資料!H8) + 發情資料!I8</f>
         <v>43326</v>
       </c>
-      <c r="F8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N8">
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8">
         <v>7</v>
       </c>
-      <c r="O8">
+      <c r="I8">
         <v>189</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="J8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="str" cm="1">
-        <f t="array" ref="A9">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N9), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N9), INDEX(基本資料!$C$51:$C$101, 配種資料!N9))</f>
+        <f t="array" ref="A9">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H9), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H9), INDEX(基本資料!$C$51:$C$101, 發情資料!H9))</f>
         <v>18Y1735-6</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" cm="1">
-        <f t="array" ref="D9">INDEX(基本資料!$E$51:$E$101, 配種資料!N9) + 配種資料!O9</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" cm="1">
+        <f t="array" ref="C9">INDEX(基本資料!$E$51:$E$101, 發情資料!H9) + 發情資料!I9</f>
         <v>43483</v>
       </c>
-      <c r="F9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N9">
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9">
         <v>8</v>
       </c>
-      <c r="O9">
+      <c r="I9">
         <v>188</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="J9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="str" cm="1">
-        <f t="array" ref="A10">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N10), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N10), INDEX(基本資料!$C$51:$C$101, 配種資料!N10))</f>
+        <f t="array" ref="A10">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H10), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H10), INDEX(基本資料!$C$51:$C$101, 發情資料!H10))</f>
         <v>18Y1735-6</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" cm="1">
-        <f t="array" ref="D10">INDEX(基本資料!$E$51:$E$101, 配種資料!N10) + 配種資料!O10</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" cm="1">
+        <f t="array" ref="C10">INDEX(基本資料!$E$51:$E$101, 發情資料!H10) + 發情資料!I10</f>
         <v>43672</v>
       </c>
-      <c r="F10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N10">
+      <c r="D10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10">
         <v>8</v>
       </c>
-      <c r="O10">
+      <c r="I10">
         <v>377</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="J10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="str" cm="1">
-        <f t="array" ref="A11">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N11), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N11), INDEX(基本資料!$C$51:$C$101, 配種資料!N11))</f>
+        <f t="array" ref="A11">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H11), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H11), INDEX(基本資料!$C$51:$C$101, 發情資料!H11))</f>
         <v>18Y1735-6</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D11" s="1" cm="1">
-        <f t="array" ref="D11">INDEX(基本資料!$E$51:$E$101, 配種資料!N11) + 配種資料!O11</f>
+      <c r="C11" s="1" cm="1">
+        <f t="array" ref="C11">INDEX(基本資料!$E$51:$E$101, 發情資料!H11) + 發情資料!I11</f>
         <v>43861</v>
       </c>
-      <c r="F11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N11">
+      <c r="D11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11">
         <v>8</v>
       </c>
-      <c r="O11">
+      <c r="I11">
         <v>566</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="J11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="str" cm="1">
-        <f t="array" ref="A12">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N12), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N12), INDEX(基本資料!$C$51:$C$101, 配種資料!N12))</f>
+        <f t="array" ref="A12">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H12), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H12), INDEX(基本資料!$C$51:$C$101, 發情資料!H12))</f>
         <v>18Y1735-6</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D12" s="1" cm="1">
-        <f t="array" ref="D12">INDEX(基本資料!$E$51:$E$101, 配種資料!N12) + 配種資料!O12</f>
+      <c r="C12" s="1" cm="1">
+        <f t="array" ref="C12">INDEX(基本資料!$E$51:$E$101, 發情資料!H12) + 發情資料!I12</f>
         <v>44049</v>
       </c>
-      <c r="F12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N12">
+      <c r="D12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12">
         <v>8</v>
       </c>
-      <c r="O12">
+      <c r="I12">
         <v>754</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="J12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="str" cm="1">
-        <f t="array" ref="A13">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N13), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N13), INDEX(基本資料!$C$51:$C$101, 配種資料!N13))</f>
+        <f t="array" ref="A13">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H13), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H13), INDEX(基本資料!$C$51:$C$101, 發情資料!H13))</f>
         <v>15Y1169-3</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" cm="1">
-        <f t="array" ref="D13">INDEX(基本資料!$E$51:$E$101, 配種資料!N13) + 配種資料!O13</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" cm="1">
+        <f t="array" ref="C13">INDEX(基本資料!$E$51:$E$101, 發情資料!H13) + 發情資料!I13</f>
         <v>42370</v>
       </c>
-      <c r="F13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N13">
+      <c r="D13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13">
         <v>9</v>
       </c>
-      <c r="O13">
+      <c r="I13">
         <v>181</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="J13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="str" cm="1">
-        <f t="array" ref="A14">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N14), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N14), INDEX(基本資料!$C$51:$C$101, 配種資料!N14))</f>
+        <f t="array" ref="A14">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H14), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H14), INDEX(基本資料!$C$51:$C$101, 發情資料!H14))</f>
         <v>18L1813-15</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" cm="1">
-        <f t="array" ref="D14">INDEX(基本資料!$E$51:$E$101, 配種資料!N14) + 配種資料!O14</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" cm="1">
+        <f t="array" ref="C14">INDEX(基本資料!$E$51:$E$101, 發情資料!H14) + 發情資料!I14</f>
         <v>43542</v>
       </c>
-      <c r="F14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N14">
+      <c r="D14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14">
         <v>10</v>
       </c>
-      <c r="O14">
+      <c r="I14">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="J14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="str" cm="1">
-        <f t="array" ref="A15">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N15), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N15), INDEX(基本資料!$C$51:$C$101, 配種資料!N15))</f>
+        <f t="array" ref="A15">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H15), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H15), INDEX(基本資料!$C$51:$C$101, 發情資料!H15))</f>
         <v>20L1665-14</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" cm="1">
-        <f t="array" ref="D15">INDEX(基本資料!$E$51:$E$101, 配種資料!N15) + 配種資料!O15</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" cm="1">
+        <f t="array" ref="C15">INDEX(基本資料!$E$51:$E$101, 發情資料!H15) + 發情資料!I15</f>
         <v>44088</v>
       </c>
-      <c r="F15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N15">
+      <c r="D15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15">
         <v>13</v>
       </c>
-      <c r="O15">
+      <c r="I15">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="J15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="str" cm="1">
-        <f t="array" ref="A16">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N16), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N16), INDEX(基本資料!$C$51:$C$101, 配種資料!N16))</f>
+        <f t="array" ref="A16">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H16), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H16), INDEX(基本資料!$C$51:$C$101, 發情資料!H16))</f>
         <v>20L1665-14</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" cm="1">
-        <f t="array" ref="D16">INDEX(基本資料!$E$51:$E$101, 配種資料!N16) + 配種資料!O16</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" cm="1">
+        <f t="array" ref="C16">INDEX(基本資料!$E$51:$E$101, 發情資料!H16) + 發情資料!I16</f>
         <v>44269</v>
       </c>
-      <c r="F16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N16">
+      <c r="D16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16">
         <v>13</v>
       </c>
-      <c r="O16">
+      <c r="I16">
         <v>368</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="J16">
+        <f t="shared" ca="1" si="0"/>
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="str" cm="1">
-        <f t="array" ref="A17">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N17), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N17), INDEX(基本資料!$C$51:$C$101, 配種資料!N17))</f>
+        <f t="array" ref="A17">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H17), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H17), INDEX(基本資料!$C$51:$C$101, 發情資料!H17))</f>
         <v>19L1292-15</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" cm="1">
-        <f t="array" ref="D17">INDEX(基本資料!$E$51:$E$101, 配種資料!N17) + 配種資料!O17</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" cm="1">
+        <f t="array" ref="C17">INDEX(基本資料!$E$51:$E$101, 發情資料!H17) + 發情資料!I17</f>
         <v>43758</v>
       </c>
-      <c r="F17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N17">
+      <c r="D17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17">
         <v>14</v>
       </c>
-      <c r="O17">
+      <c r="I17">
         <v>187</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="J17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="str" cm="1">
-        <f t="array" ref="A18">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N18), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N18), INDEX(基本資料!$C$51:$C$101, 配種資料!N18))</f>
+        <f t="array" ref="A18">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H18), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H18), INDEX(基本資料!$C$51:$C$101, 發情資料!H18))</f>
         <v>19L1292-15</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D18" s="1" cm="1">
-        <f t="array" ref="D18">INDEX(基本資料!$E$51:$E$101, 配種資料!N18) + 配種資料!O18</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" cm="1">
+        <f t="array" ref="C18">INDEX(基本資料!$E$51:$E$101, 發情資料!H18) + 發情資料!I18</f>
         <v>43944</v>
       </c>
-      <c r="F18" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N18">
+      <c r="D18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18">
         <v>14</v>
       </c>
-      <c r="O18">
+      <c r="I18">
         <v>373</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="J18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="str" cm="1">
-        <f t="array" ref="A19">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N19), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N19), INDEX(基本資料!$C$51:$C$101, 配種資料!N19))</f>
+        <f t="array" ref="A19">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H19), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H19), INDEX(基本資料!$C$51:$C$101, 發情資料!H19))</f>
         <v>19L1292-15</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D19" s="1" cm="1">
-        <f t="array" ref="D19">INDEX(基本資料!$E$51:$E$101, 配種資料!N19) + 配種資料!O19</f>
+      <c r="C19" s="1" cm="1">
+        <f t="array" ref="C19">INDEX(基本資料!$E$51:$E$101, 發情資料!H19) + 發情資料!I19</f>
         <v>44128</v>
       </c>
-      <c r="F19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N19">
+      <c r="D19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19">
         <v>14</v>
       </c>
-      <c r="O19">
+      <c r="I19">
         <v>557</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="J19">
+        <f t="shared" ca="1" si="0"/>
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="str" cm="1">
-        <f t="array" ref="A20">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N20), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N20), INDEX(基本資料!$C$51:$C$101, 配種資料!N20))</f>
+        <f t="array" ref="A20">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H20), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H20), INDEX(基本資料!$C$51:$C$101, 發情資料!H20))</f>
         <v>19L1292-15</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D20" s="1" cm="1">
-        <f t="array" ref="D20">INDEX(基本資料!$E$51:$E$101, 配種資料!N20) + 配種資料!O20</f>
+      <c r="C20" s="1" cm="1">
+        <f t="array" ref="C20">INDEX(基本資料!$E$51:$E$101, 發情資料!H20) + 發情資料!I20</f>
         <v>44318</v>
       </c>
-      <c r="F20" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N20">
+      <c r="D20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20">
         <v>14</v>
       </c>
-      <c r="O20">
+      <c r="I20">
         <v>747</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="J20">
+        <f t="shared" ca="1" si="0"/>
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="str" cm="1">
-        <f t="array" ref="A21">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N21), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N21), INDEX(基本資料!$C$51:$C$101, 配種資料!N21))</f>
+        <f t="array" ref="A21">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H21), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H21), INDEX(基本資料!$C$51:$C$101, 發情資料!H21))</f>
         <v>23L1286-4</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" cm="1">
-        <f t="array" ref="D21">INDEX(基本資料!$E$51:$E$101, 配種資料!N21) + 配種資料!O21</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" cm="1">
+        <f t="array" ref="C21">INDEX(基本資料!$E$51:$E$101, 發情資料!H21) + 發情資料!I21</f>
         <v>45412</v>
       </c>
-      <c r="F21" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N21">
+      <c r="D21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21">
         <v>15</v>
       </c>
-      <c r="O21">
+      <c r="I21">
         <v>181</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="J21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="str" cm="1">
-        <f t="array" ref="A22">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N22), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N22), INDEX(基本資料!$C$51:$C$101, 配種資料!N22))</f>
+        <f t="array" ref="A22">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H22), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H22), INDEX(基本資料!$C$51:$C$101, 發情資料!H22))</f>
         <v>20L1580-5</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" cm="1">
-        <f t="array" ref="D22">INDEX(基本資料!$E$51:$E$101, 配種資料!N22) + 配種資料!O22</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" cm="1">
+        <f t="array" ref="C22">INDEX(基本資料!$E$51:$E$101, 發情資料!H22) + 發情資料!I22</f>
         <v>44136</v>
       </c>
-      <c r="F22" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N22">
+      <c r="D22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22">
         <v>16</v>
       </c>
-      <c r="O22">
+      <c r="I22">
         <v>188</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="J22">
+        <f t="shared" ca="1" si="0"/>
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="str" cm="1">
-        <f t="array" ref="A23">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N23), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N23), INDEX(基本資料!$C$51:$C$101, 配種資料!N23))</f>
+        <f t="array" ref="A23">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H23), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H23), INDEX(基本資料!$C$51:$C$101, 發情資料!H23))</f>
         <v>20L1580-5</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D23" s="1" cm="1">
-        <f t="array" ref="D23">INDEX(基本資料!$E$51:$E$101, 配種資料!N23) + 配種資料!O23</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" cm="1">
+        <f t="array" ref="C23">INDEX(基本資料!$E$51:$E$101, 發情資料!H23) + 發情資料!I23</f>
         <v>44318</v>
       </c>
-      <c r="F23" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N23">
+      <c r="D23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23">
         <v>16</v>
       </c>
-      <c r="O23">
+      <c r="I23">
         <v>370</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="J23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="str" cm="1">
-        <f t="array" ref="A24">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N24), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N24), INDEX(基本資料!$C$51:$C$101, 配種資料!N24))</f>
+        <f t="array" ref="A24">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H24), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H24), INDEX(基本資料!$C$51:$C$101, 發情資料!H24))</f>
         <v>22D1440-12</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" cm="1">
-        <f t="array" ref="D24">INDEX(基本資料!$E$51:$E$101, 配種資料!N24) + 配種資料!O24</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" cm="1">
+        <f t="array" ref="C24">INDEX(基本資料!$E$51:$E$101, 發情資料!H24) + 發情資料!I24</f>
         <v>45107</v>
       </c>
-      <c r="F24" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N24">
+      <c r="D24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24">
         <v>17</v>
       </c>
-      <c r="O24">
+      <c r="I24">
         <v>187</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="J24">
+        <f t="shared" ca="1" si="0"/>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="str" cm="1">
-        <f t="array" ref="A25">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N25), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N25), INDEX(基本資料!$C$51:$C$101, 配種資料!N25))</f>
+        <f t="array" ref="A25">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H25), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H25), INDEX(基本資料!$C$51:$C$101, 發情資料!H25))</f>
         <v>22D1440-12</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D25" s="1" cm="1">
-        <f t="array" ref="D25">INDEX(基本資料!$E$51:$E$101, 配種資料!N25) + 配種資料!O25</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" cm="1">
+        <f t="array" ref="C25">INDEX(基本資料!$E$51:$E$101, 發情資料!H25) + 發情資料!I25</f>
         <v>45297</v>
       </c>
-      <c r="F25" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N25">
+      <c r="D25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25">
         <v>17</v>
       </c>
-      <c r="O25">
+      <c r="I25">
         <v>377</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="J25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="str" cm="1">
-        <f t="array" ref="A26">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N26), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N26), INDEX(基本資料!$C$51:$C$101, 配種資料!N26))</f>
+        <f t="array" ref="A26">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H26), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H26), INDEX(基本資料!$C$51:$C$101, 發情資料!H26))</f>
         <v>21L1512-9</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" cm="1">
-        <f t="array" ref="D26">INDEX(基本資料!$E$51:$E$101, 配種資料!N26) + 配種資料!O26</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" cm="1">
+        <f t="array" ref="C26">INDEX(基本資料!$E$51:$E$101, 發情資料!H26) + 發情資料!I26</f>
         <v>44517</v>
       </c>
-      <c r="F26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N26">
+      <c r="D26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H26">
         <v>18</v>
       </c>
-      <c r="O26">
+      <c r="I26">
         <v>187</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="J26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="str" cm="1">
-        <f t="array" ref="A27">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N27), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N27), INDEX(基本資料!$C$51:$C$101, 配種資料!N27))</f>
+        <f t="array" ref="A27">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H27), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H27), INDEX(基本資料!$C$51:$C$101, 發情資料!H27))</f>
         <v>22D1284-7</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" cm="1">
-        <f t="array" ref="D27">INDEX(基本資料!$E$51:$E$101, 配種資料!N27) + 配種資料!O27</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" cm="1">
+        <f t="array" ref="C27">INDEX(基本資料!$E$51:$E$101, 發情資料!H27) + 發情資料!I27</f>
         <v>44951</v>
       </c>
-      <c r="F27" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N27">
-        <v>19</v>
-      </c>
-      <c r="O27">
+      <c r="D27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" t="s">
+        <v>131</v>
+      </c>
+      <c r="H27">
+        <v>19</v>
+      </c>
+      <c r="I27">
         <v>183</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="J27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="str" cm="1">
-        <f t="array" ref="A28">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N28), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N28), INDEX(基本資料!$C$51:$C$101, 配種資料!N28))</f>
+        <f t="array" ref="A28">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H28), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H28), INDEX(基本資料!$C$51:$C$101, 發情資料!H28))</f>
         <v>15Y1417-7</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" cm="1">
-        <f t="array" ref="D28">INDEX(基本資料!$E$51:$E$101, 配種資料!N28) + 配種資料!O28</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" cm="1">
+        <f t="array" ref="C28">INDEX(基本資料!$E$51:$E$101, 發情資料!H28) + 發情資料!I28</f>
         <v>42219</v>
       </c>
-      <c r="F28" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N28">
+      <c r="D28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F28" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28">
         <v>21</v>
       </c>
-      <c r="O28">
+      <c r="I28">
         <v>180</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="J28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="str" cm="1">
-        <f t="array" ref="A29">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N29), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N29), INDEX(基本資料!$C$51:$C$101, 配種資料!N29))</f>
+        <f t="array" ref="A29">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H29), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H29), INDEX(基本資料!$C$51:$C$101, 發情資料!H29))</f>
         <v>15Y1417-7</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D29" s="1" cm="1">
-        <f t="array" ref="D29">INDEX(基本資料!$E$51:$E$101, 配種資料!N29) + 配種資料!O29</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" cm="1">
+        <f t="array" ref="C29">INDEX(基本資料!$E$51:$E$101, 發情資料!H29) + 發情資料!I29</f>
         <v>42406</v>
       </c>
-      <c r="F29" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N29">
+      <c r="D29" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" t="s">
+        <v>131</v>
+      </c>
+      <c r="H29">
         <v>21</v>
       </c>
-      <c r="O29">
+      <c r="I29">
         <v>367</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="J29">
+        <f t="shared" ca="1" si="0"/>
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="str" cm="1">
-        <f t="array" ref="A30">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N30), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N30), INDEX(基本資料!$C$51:$C$101, 配種資料!N30))</f>
+        <f t="array" ref="A30">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H30), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H30), INDEX(基本資料!$C$51:$C$101, 發情資料!H30))</f>
         <v>23L1910-17</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" cm="1">
-        <f t="array" ref="D30">INDEX(基本資料!$E$51:$E$101, 配種資料!N30) + 配種資料!O30</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" cm="1">
+        <f t="array" ref="C30">INDEX(基本資料!$E$51:$E$101, 發情資料!H30) + 發情資料!I30</f>
         <v>45122</v>
       </c>
-      <c r="F30" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N30">
+      <c r="D30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" t="s">
+        <v>131</v>
+      </c>
+      <c r="H30">
         <v>22</v>
       </c>
-      <c r="O30">
+      <c r="I30">
         <v>180</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="J30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="str" cm="1">
-        <f t="array" ref="A31">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N31), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N31), INDEX(基本資料!$C$51:$C$101, 配種資料!N31))</f>
+        <f t="array" ref="A31">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H31), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H31), INDEX(基本資料!$C$51:$C$101, 發情資料!H31))</f>
         <v>23L1910-17</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D31" s="1" cm="1">
-        <f t="array" ref="D31">INDEX(基本資料!$E$51:$E$101, 配種資料!N31) + 配種資料!O31</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" cm="1">
+        <f t="array" ref="C31">INDEX(基本資料!$E$51:$E$101, 發情資料!H31) + 發情資料!I31</f>
         <v>45304</v>
       </c>
-      <c r="F31" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N31">
+      <c r="D31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" t="s">
+        <v>131</v>
+      </c>
+      <c r="H31">
         <v>22</v>
       </c>
-      <c r="O31">
+      <c r="I31">
         <v>362</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="J31">
+        <f t="shared" ca="1" si="0"/>
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="str" cm="1">
-        <f t="array" ref="A32">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N32), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N32), INDEX(基本資料!$C$51:$C$101, 配種資料!N32))</f>
+        <f t="array" ref="A32">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H32), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H32), INDEX(基本資料!$C$51:$C$101, 發情資料!H32))</f>
         <v>16L1961-5</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" cm="1">
-        <f t="array" ref="D32">INDEX(基本資料!$E$51:$E$101, 配種資料!N32) + 配種資料!O32</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" cm="1">
+        <f t="array" ref="C32">INDEX(基本資料!$E$51:$E$101, 發情資料!H32) + 發情資料!I32</f>
         <v>42625</v>
       </c>
-      <c r="F32" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N32">
+      <c r="D32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32">
         <v>23</v>
       </c>
-      <c r="O32">
+      <c r="I32">
         <v>188</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="J32">
+        <f t="shared" ca="1" si="0"/>
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="str" cm="1">
-        <f t="array" ref="A33">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N33), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N33), INDEX(基本資料!$C$51:$C$101, 配種資料!N33))</f>
+        <f t="array" ref="A33">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H33), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H33), INDEX(基本資料!$C$51:$C$101, 發情資料!H33))</f>
         <v>18D1565-10</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" cm="1">
-        <f t="array" ref="D33">INDEX(基本資料!$E$51:$E$101, 配種資料!N33) + 配種資料!O33</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" cm="1">
+        <f t="array" ref="C33">INDEX(基本資料!$E$51:$E$101, 發情資料!H33) + 發情資料!I33</f>
         <v>43635</v>
       </c>
-      <c r="F33" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N33">
+      <c r="D33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33">
         <v>24</v>
       </c>
-      <c r="O33">
+      <c r="I33">
         <v>186</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="J33">
+        <f t="shared" ca="1" si="0"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="str" cm="1">
-        <f t="array" ref="A34">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N34), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N34), INDEX(基本資料!$C$51:$C$101, 配種資料!N34))</f>
+        <f t="array" ref="A34">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H34), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H34), INDEX(基本資料!$C$51:$C$101, 發情資料!H34))</f>
         <v>18D1565-10</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D34" s="1" cm="1">
-        <f t="array" ref="D34">INDEX(基本資料!$E$51:$E$101, 配種資料!N34) + 配種資料!O34</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" cm="1">
+        <f t="array" ref="C34">INDEX(基本資料!$E$51:$E$101, 發情資料!H34) + 發情資料!I34</f>
         <v>43824</v>
       </c>
-      <c r="F34" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N34">
+      <c r="D34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34">
         <v>24</v>
       </c>
-      <c r="O34">
+      <c r="I34">
         <v>375</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="J34">
+        <f t="shared" ca="1" si="0"/>
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="str" cm="1">
-        <f t="array" ref="A35">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N35), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N35), INDEX(基本資料!$C$51:$C$101, 配種資料!N35))</f>
+        <f t="array" ref="A35">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H35), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H35), INDEX(基本資料!$C$51:$C$101, 發情資料!H35))</f>
         <v>18D1565-10</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D35" s="1" cm="1">
-        <f t="array" ref="D35">INDEX(基本資料!$E$51:$E$101, 配種資料!N35) + 配種資料!O35</f>
+      <c r="C35" s="1" cm="1">
+        <f t="array" ref="C35">INDEX(基本資料!$E$51:$E$101, 發情資料!H35) + 發情資料!I35</f>
         <v>44009</v>
       </c>
-      <c r="F35" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N35">
+      <c r="D35" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35">
         <v>24</v>
       </c>
-      <c r="O35">
+      <c r="I35">
         <v>560</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="J35">
+        <f t="shared" ca="1" si="0"/>
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="str" cm="1">
-        <f t="array" ref="A36">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N36), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N36), INDEX(基本資料!$C$51:$C$101, 配種資料!N36))</f>
+        <f t="array" ref="A36">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H36), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H36), INDEX(基本資料!$C$51:$C$101, 發情資料!H36))</f>
         <v>20L1966-4</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D36" s="1" cm="1">
-        <f t="array" ref="D36">INDEX(基本資料!$E$51:$E$101, 配種資料!N36) + 配種資料!O36</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" cm="1">
+        <f t="array" ref="C36">INDEX(基本資料!$E$51:$E$101, 發情資料!H36) + 發情資料!I36</f>
         <v>44066</v>
       </c>
-      <c r="F36" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N36">
+      <c r="D36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36">
         <v>26</v>
       </c>
-      <c r="O36">
+      <c r="I36">
         <v>181</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="J36">
+        <f t="shared" ca="1" si="0"/>
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="str" cm="1">
-        <f t="array" ref="A37">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N37), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N37), INDEX(基本資料!$C$51:$C$101, 配種資料!N37))</f>
+        <f t="array" ref="A37">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H37), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H37), INDEX(基本資料!$C$51:$C$101, 發情資料!H37))</f>
         <v>22Y1106-1</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D37" s="1" cm="1">
-        <f t="array" ref="D37">INDEX(基本資料!$E$51:$E$101, 配種資料!N37) + 配種資料!O37</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" cm="1">
+        <f t="array" ref="C37">INDEX(基本資料!$E$51:$E$101, 發情資料!H37) + 發情資料!I37</f>
         <v>45009</v>
       </c>
-      <c r="F37" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N37">
+      <c r="D37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" t="s">
+        <v>131</v>
+      </c>
+      <c r="H37">
         <v>27</v>
       </c>
-      <c r="O37">
+      <c r="I37">
         <v>181</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="J37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="str" cm="1">
-        <f t="array" ref="A38">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N38), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N38), INDEX(基本資料!$C$51:$C$101, 配種資料!N38))</f>
+        <f t="array" ref="A38">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H38), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H38), INDEX(基本資料!$C$51:$C$101, 發情資料!H38))</f>
         <v>20L1782-4</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D38" s="1" cm="1">
-        <f t="array" ref="D38">INDEX(基本資料!$E$51:$E$101, 配種資料!N38) + 配種資料!O38</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" cm="1">
+        <f t="array" ref="C38">INDEX(基本資料!$E$51:$E$101, 發情資料!H38) + 發情資料!I38</f>
         <v>44205</v>
       </c>
-      <c r="F38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N38">
+      <c r="D38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" t="s">
+        <v>131</v>
+      </c>
+      <c r="H38">
         <v>29</v>
       </c>
-      <c r="O38">
+      <c r="I38">
         <v>184</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="J38">
+        <f t="shared" ca="1" si="0"/>
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="str" cm="1">
-        <f t="array" ref="A39">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N39), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N39), INDEX(基本資料!$C$51:$C$101, 配種資料!N39))</f>
+        <f t="array" ref="A39">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H39), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H39), INDEX(基本資料!$C$51:$C$101, 發情資料!H39))</f>
         <v>24L1547-2</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D39" s="1" cm="1">
-        <f t="array" ref="D39">INDEX(基本資料!$E$51:$E$101, 配種資料!N39) + 配種資料!O39</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" cm="1">
+        <f t="array" ref="C39">INDEX(基本資料!$E$51:$E$101, 發情資料!H39) + 發情資料!I39</f>
         <v>45753</v>
       </c>
-      <c r="F39" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N39">
+      <c r="D39" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
+        <v>131</v>
+      </c>
+      <c r="H39">
         <v>30</v>
       </c>
-      <c r="O39">
+      <c r="I39">
         <v>182</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="J39">
+        <f t="shared" ca="1" si="0"/>
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="str" cm="1">
-        <f t="array" ref="A40">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N40), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N40), INDEX(基本資料!$C$51:$C$101, 配種資料!N40))</f>
+        <f t="array" ref="A40">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H40), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H40), INDEX(基本資料!$C$51:$C$101, 發情資料!H40))</f>
         <v>24L1547-2</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D40" s="1" cm="1">
-        <f t="array" ref="D40">INDEX(基本資料!$E$51:$E$101, 配種資料!N40) + 配種資料!O40</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" cm="1">
+        <f t="array" ref="C40">INDEX(基本資料!$E$51:$E$101, 發情資料!H40) + 發情資料!I40</f>
         <v>45941</v>
       </c>
-      <c r="F40" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N40">
+      <c r="D40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>131</v>
+      </c>
+      <c r="F40" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40">
         <v>30</v>
       </c>
-      <c r="O40">
+      <c r="I40">
         <v>370</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="J40">
+        <f t="shared" ca="1" si="0"/>
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="str" cm="1">
-        <f t="array" ref="A41">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N41), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N41), INDEX(基本資料!$C$51:$C$101, 配種資料!N41))</f>
+        <f t="array" ref="A41">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H41), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H41), INDEX(基本資料!$C$51:$C$101, 發情資料!H41))</f>
         <v>24L1547-2</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D41" s="1" cm="1">
-        <f t="array" ref="D41">INDEX(基本資料!$E$51:$E$101, 配種資料!N41) + 配種資料!O41</f>
+      <c r="C41" s="1" cm="1">
+        <f t="array" ref="C41">INDEX(基本資料!$E$51:$E$101, 發情資料!H41) + 發情資料!I41</f>
         <v>46122</v>
       </c>
-      <c r="F41" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N41">
+      <c r="D41" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" t="s">
+        <v>131</v>
+      </c>
+      <c r="H41">
         <v>30</v>
       </c>
-      <c r="O41">
+      <c r="I41">
         <v>551</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="J41">
+        <f t="shared" ca="1" si="0"/>
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="str" cm="1">
-        <f t="array" ref="A42">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N42), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N42), INDEX(基本資料!$C$51:$C$101, 配種資料!N42))</f>
+        <f t="array" ref="A42">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H42), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H42), INDEX(基本資料!$C$51:$C$101, 發情資料!H42))</f>
         <v>24D1947-13</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" cm="1">
-        <f t="array" ref="D42">INDEX(基本資料!$E$51:$E$101, 配種資料!N42) + 配種資料!O42</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" cm="1">
+        <f t="array" ref="C42">INDEX(基本資料!$E$51:$E$101, 發情資料!H42) + 發情資料!I42</f>
         <v>45764</v>
       </c>
-      <c r="F42" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N42">
+      <c r="D42" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42">
         <v>32</v>
       </c>
-      <c r="O42">
+      <c r="I42">
         <v>182</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="J42">
+        <f t="shared" ca="1" si="0"/>
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="str" cm="1">
-        <f t="array" ref="A43">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N43), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N43), INDEX(基本資料!$C$51:$C$101, 配種資料!N43))</f>
+        <f t="array" ref="A43">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H43), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H43), INDEX(基本資料!$C$51:$C$101, 發情資料!H43))</f>
         <v>21D1472-1</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" cm="1">
-        <f t="array" ref="D43">INDEX(基本資料!$E$51:$E$101, 配種資料!N43) + 配種資料!O43</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" cm="1">
+        <f t="array" ref="C43">INDEX(基本資料!$E$51:$E$101, 發情資料!H43) + 發情資料!I43</f>
         <v>44623</v>
       </c>
-      <c r="F43" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N43">
+      <c r="D43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43">
         <v>33</v>
       </c>
-      <c r="O43">
+      <c r="I43">
         <v>189</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="J43">
+        <f t="shared" ca="1" si="0"/>
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="str" cm="1">
-        <f t="array" ref="A44">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N44), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N44), INDEX(基本資料!$C$51:$C$101, 配種資料!N44))</f>
+        <f t="array" ref="A44">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H44), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H44), INDEX(基本資料!$C$51:$C$101, 發情資料!H44))</f>
         <v>21D1472-1</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D44" s="1" cm="1">
-        <f t="array" ref="D44">INDEX(基本資料!$E$51:$E$101, 配種資料!N44) + 配種資料!O44</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" cm="1">
+        <f t="array" ref="C44">INDEX(基本資料!$E$51:$E$101, 發情資料!H44) + 發情資料!I44</f>
         <v>44812</v>
       </c>
-      <c r="F44" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N44">
+      <c r="D44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" t="s">
+        <v>131</v>
+      </c>
+      <c r="H44">
         <v>33</v>
       </c>
-      <c r="O44">
+      <c r="I44">
         <v>378</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="J44">
+        <f t="shared" ca="1" si="0"/>
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="str" cm="1">
-        <f t="array" ref="A45">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N45), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N45), INDEX(基本資料!$C$51:$C$101, 配種資料!N45))</f>
+        <f t="array" ref="A45">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H45), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H45), INDEX(基本資料!$C$51:$C$101, 發情資料!H45))</f>
         <v>23D1122-4</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D45" s="1" cm="1">
-        <f t="array" ref="D45">INDEX(基本資料!$E$51:$E$101, 配種資料!N45) + 配種資料!O45</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" cm="1">
+        <f t="array" ref="C45">INDEX(基本資料!$E$51:$E$101, 發情資料!H45) + 發情資料!I45</f>
         <v>45290</v>
       </c>
-      <c r="F45" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N45">
+      <c r="D45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45" t="s">
+        <v>131</v>
+      </c>
+      <c r="H45">
         <v>34</v>
       </c>
-      <c r="O45">
+      <c r="I45">
         <v>182</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="J45">
+        <f t="shared" ca="1" si="0"/>
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="str" cm="1">
-        <f t="array" ref="A46">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N46), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N46), INDEX(基本資料!$C$51:$C$101, 配種資料!N46))</f>
+        <f t="array" ref="A46">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H46), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H46), INDEX(基本資料!$C$51:$C$101, 發情資料!H46))</f>
         <v>23D1122-4</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D46" s="1" cm="1">
-        <f t="array" ref="D46">INDEX(基本資料!$E$51:$E$101, 配種資料!N46) + 配種資料!O46</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" cm="1">
+        <f t="array" ref="C46">INDEX(基本資料!$E$51:$E$101, 發情資料!H46) + 發情資料!I46</f>
         <v>45474</v>
       </c>
-      <c r="F46" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N46">
+      <c r="D46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+      <c r="F46" t="s">
+        <v>131</v>
+      </c>
+      <c r="H46">
         <v>34</v>
       </c>
-      <c r="O46">
+      <c r="I46">
         <v>366</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="J46">
+        <f t="shared" ca="1" si="0"/>
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="str" cm="1">
-        <f t="array" ref="A47">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N47), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N47), INDEX(基本資料!$C$51:$C$101, 配種資料!N47))</f>
+        <f t="array" ref="A47">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H47), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H47), INDEX(基本資料!$C$51:$C$101, 發情資料!H47))</f>
         <v>19D1457-11</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D47" s="1" cm="1">
-        <f t="array" ref="D47">INDEX(基本資料!$E$51:$E$101, 配種資料!N47) + 配種資料!O47</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" cm="1">
+        <f t="array" ref="C47">INDEX(基本資料!$E$51:$E$101, 發情資料!H47) + 發情資料!I47</f>
         <v>43843</v>
       </c>
-      <c r="F47" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N47">
+      <c r="D47" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" t="s">
+        <v>131</v>
+      </c>
+      <c r="H47">
         <v>35</v>
       </c>
-      <c r="O47">
+      <c r="I47">
         <v>181</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="J47">
+        <f t="shared" ca="1" si="0"/>
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="str" cm="1">
-        <f t="array" ref="A48">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N48), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N48), INDEX(基本資料!$C$51:$C$101, 配種資料!N48))</f>
+        <f t="array" ref="A48">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H48), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H48), INDEX(基本資料!$C$51:$C$101, 發情資料!H48))</f>
         <v>16D1988-11</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D48" s="1" cm="1">
-        <f t="array" ref="D48">INDEX(基本資料!$E$51:$E$101, 配種資料!N48) + 配種資料!O48</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" cm="1">
+        <f t="array" ref="C48">INDEX(基本資料!$E$51:$E$101, 發情資料!H48) + 發情資料!I48</f>
         <v>42857</v>
       </c>
-      <c r="F48" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N48">
+      <c r="D48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48">
         <v>39</v>
       </c>
-      <c r="O48">
+      <c r="I48">
         <v>189</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="J48">
+        <f t="shared" ca="1" si="0"/>
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="str" cm="1">
-        <f t="array" ref="A49">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N49), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N49), INDEX(基本資料!$C$51:$C$101, 配種資料!N49))</f>
+        <f t="array" ref="A49">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H49), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H49), INDEX(基本資料!$C$51:$C$101, 發情資料!H49))</f>
         <v>19Y1792-14</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D49" s="1" cm="1">
-        <f t="array" ref="D49">INDEX(基本資料!$E$51:$E$101, 配種資料!N49) + 配種資料!O49</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" cm="1">
+        <f t="array" ref="C49">INDEX(基本資料!$E$51:$E$101, 發情資料!H49) + 發情資料!I49</f>
         <v>43837</v>
       </c>
-      <c r="F49" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N49">
+      <c r="D49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" t="s">
+        <v>131</v>
+      </c>
+      <c r="H49">
         <v>43</v>
       </c>
-      <c r="O49">
+      <c r="I49">
         <v>182</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="J49">
+        <f t="shared" ca="1" si="0"/>
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="str" cm="1">
-        <f t="array" ref="A50">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N50), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N50), INDEX(基本資料!$C$51:$C$101, 配種資料!N50))</f>
+        <f t="array" ref="A50">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H50), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H50), INDEX(基本資料!$C$51:$C$101, 發情資料!H50))</f>
         <v>17D1288-6</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" cm="1">
-        <f t="array" ref="D50">INDEX(基本資料!$E$51:$E$101, 配種資料!N50) + 配種資料!O50</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" cm="1">
+        <f t="array" ref="C50">INDEX(基本資料!$E$51:$E$101, 發情資料!H50) + 發情資料!I50</f>
         <v>42933</v>
       </c>
-      <c r="F50" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N50">
+      <c r="D50" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" t="s">
+        <v>131</v>
+      </c>
+      <c r="H50">
         <v>48</v>
       </c>
-      <c r="O50">
+      <c r="I50">
         <v>190</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="J50">
+        <f t="shared" ca="1" si="0"/>
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="str" cm="1">
-        <f t="array" ref="A51">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 配種資料!N51), "YY"), INDEX(基本資料!$B$51:$B$101, 配種資料!N51), INDEX(基本資料!$C$51:$C$101, 配種資料!N51))</f>
+        <f t="array" ref="A51">_xlfn.CONCAT(TEXT(INDEX(基本資料!$E$51:$E$101, 發情資料!H51), "YY"), INDEX(基本資料!$B$51:$B$101, 發情資料!H51), INDEX(基本資料!$C$51:$C$101, 發情資料!H51))</f>
         <v>20Y1171-6</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D51" s="1" cm="1">
-        <f t="array" ref="D51">INDEX(基本資料!$E$51:$E$101, 配種資料!N51) + 配種資料!O51</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" cm="1">
+        <f t="array" ref="C51">INDEX(基本資料!$E$51:$E$101, 發情資料!H51) + 發情資料!I51</f>
         <v>44291</v>
       </c>
-      <c r="F51" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N51">
+      <c r="D51" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" t="s">
+        <v>131</v>
+      </c>
+      <c r="H51">
         <v>50</v>
       </c>
-      <c r="O51">
+      <c r="I51">
         <v>185</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="J51">
+        <f t="shared" ca="1" si="0"/>
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>117106</v>
       </c>
       <c r="B52">
         <v>4</v>
       </c>
-      <c r="D52" s="1">
+      <c r="C52" s="1">
         <v>44474</v>
       </c>
-      <c r="F52" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L52" t="s">
+      <c r="D52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>131</v>
+      </c>
+      <c r="F52" t="s">
+        <v>131</v>
+      </c>
+      <c r="G52" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52">
+        <f t="shared" ca="1" si="0"/>
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>44505</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F53" t="s">
+        <v>131</v>
+      </c>
+      <c r="G53" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
-      <c r="A53" t="s">
+      <c r="J53">
+        <f t="shared" ca="1" si="0"/>
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>44505</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>131</v>
+      </c>
+      <c r="F54" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" t="s">
         <v>136</v>
       </c>
-      <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="D53" s="1">
+      <c r="J54">
+        <f t="shared" ca="1" si="0"/>
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="1">
         <v>44505</v>
       </c>
-      <c r="F53" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L53" t="s">
+      <c r="D55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F55" t="s">
+        <v>131</v>
+      </c>
+      <c r="G55" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1">
-        <v>44505</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L54" t="s">
+      <c r="J55">
+        <f t="shared" ca="1" si="0"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E56" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56" t="s">
+        <v>131</v>
+      </c>
+      <c r="G56" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="1">
-        <v>44505</v>
-      </c>
-      <c r="F55" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L55" t="s">
+      <c r="J56">
+        <f t="shared" ca="1" si="0"/>
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" s="1">
+        <v>44321</v>
+      </c>
+      <c r="E57" t="s">
+        <v>131</v>
+      </c>
+      <c r="F57" t="s">
+        <v>131</v>
+      </c>
+      <c r="G57" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" t="s">
-        <v>136</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="F56" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L56" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" t="s">
-        <v>136</v>
-      </c>
-      <c r="B57">
-        <v>2</v>
-      </c>
-      <c r="D57" s="1">
-        <v>44321</v>
-      </c>
-      <c r="L57" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="J57">
+        <f t="shared" ca="1" si="0"/>
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
-      <c r="D58" s="1">
+      <c r="C58" s="1">
         <v>43590</v>
       </c>
-      <c r="F58" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L58" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="D58" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>131</v>
+      </c>
+      <c r="F58" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58" t="s">
+        <v>140</v>
+      </c>
+      <c r="J58">
+        <f t="shared" ca="1" si="0"/>
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59">
         <v>13</v>
       </c>
-      <c r="D59" s="1">
+      <c r="C59" s="1">
         <v>44505</v>
       </c>
-      <c r="F59" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L59" t="s">
-        <v>143</v>
+      <c r="D59" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G59" t="s">
+        <v>141</v>
+      </c>
+      <c r="J59">
+        <f t="shared" ca="1" si="0"/>
+        <v>1128</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O2:O1048575">
-    <sortCondition ref="O2:O1048575"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:I1048575">
+    <sortCondition ref="I2:I1048575"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add pig born litter.
</commit_message>
<xml_diff>
--- a/test/helper/estrus_data/estrus_data.xlsx
+++ b/test/helper/estrus_data/estrus_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3AEE805-1871-4325-96CE-5014DF72019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{859F09BE-B7A4-4917-ABF6-382E2C07CA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基本資料" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="143">
   <si>
     <t>序號</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>欄1</t>
+  </si>
+  <si>
+    <t>出生胎次</t>
   </si>
   <si>
     <t>D</t>
@@ -856,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -867,7 +870,7 @@
     <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.5">
+    <row r="1" spans="1:18" ht="16.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -919,13 +922,16 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="16.5">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="16.5">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1">
         <v>44832</v>
@@ -934,21 +940,21 @@
         <v>220815</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16.5">
+    <row r="3" spans="1:18" ht="16.5">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1">
         <v>45248</v>
@@ -957,21 +963,21 @@
         <v>114463</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5">
+    <row r="4" spans="1:18" ht="16.5">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>43117</v>
@@ -980,67 +986,67 @@
         <v>571977</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.5">
+    <row r="5" spans="1:18" ht="16.5">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>44774</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.5">
+    <row r="6" spans="1:18" ht="16.5">
       <c r="A6">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
         <v>45192</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.5">
+    <row r="7" spans="1:18" ht="16.5">
       <c r="A7">
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
         <v>42478</v>
@@ -1049,44 +1055,44 @@
         <v>622282</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5">
+    <row r="8" spans="1:18" ht="16.5">
       <c r="A8">
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1">
         <v>42972</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16.5">
+    <row r="9" spans="1:18" ht="16.5">
       <c r="A9">
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1">
         <v>42171</v>
@@ -1095,67 +1101,67 @@
         <v>546867</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16.5">
+    <row r="10" spans="1:18" ht="16.5">
       <c r="A10">
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1">
         <v>43264</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5">
+    <row r="11" spans="1:18" ht="16.5">
       <c r="A11">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1">
         <v>45151</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16.5">
+    <row r="12" spans="1:18" ht="16.5">
       <c r="A12">
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1">
         <v>44494</v>
@@ -1164,21 +1170,21 @@
         <v>695593</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16.5">
+    <row r="13" spans="1:18" ht="16.5">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1">
         <v>44193</v>
@@ -1187,21 +1193,21 @@
         <v>630400</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16.5">
+    <row r="14" spans="1:18" ht="16.5">
       <c r="A14">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1">
         <v>42177</v>
@@ -1210,21 +1216,21 @@
         <v>590433</v>
       </c>
       <c r="I14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16.5">
+    <row r="15" spans="1:18" ht="16.5">
       <c r="A15">
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1">
         <v>44338</v>
@@ -1233,30 +1239,30 @@
         <v>246174</v>
       </c>
       <c r="I15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="16.5">
+    <row r="16" spans="1:18" ht="16.5">
       <c r="A16">
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1">
         <v>42646</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -1267,19 +1273,19 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1">
         <v>42378</v>
       </c>
       <c r="H17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -1290,10 +1296,10 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1">
         <v>43824</v>
@@ -1302,7 +1308,7 @@
         <v>348752</v>
       </c>
       <c r="I18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1313,10 +1319,10 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" s="1">
         <v>42152</v>
@@ -1325,7 +1331,7 @@
         <v>984299</v>
       </c>
       <c r="I19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -1336,19 +1342,19 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E20" s="1">
         <v>44746</v>
       </c>
       <c r="H20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -1359,10 +1365,10 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="1">
         <v>42497</v>
@@ -1371,7 +1377,7 @@
         <v>188631</v>
       </c>
       <c r="I21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -1382,10 +1388,10 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1">
         <v>43655</v>
@@ -1394,7 +1400,7 @@
         <v>190895</v>
       </c>
       <c r="I22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -1405,10 +1411,10 @@
         <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23" s="1">
         <v>44250</v>
@@ -1417,7 +1423,7 @@
         <v>454447</v>
       </c>
       <c r="I23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1428,10 +1434,10 @@
         <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24" s="1">
         <v>42692</v>
@@ -1440,7 +1446,7 @@
         <v>822190</v>
       </c>
       <c r="I24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -1451,10 +1457,10 @@
         <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E25" s="1">
         <v>42243</v>
@@ -1463,7 +1469,7 @@
         <v>178181</v>
       </c>
       <c r="I25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -1474,10 +1480,10 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E26" s="1">
         <v>42329</v>
@@ -1486,7 +1492,7 @@
         <v>706220</v>
       </c>
       <c r="I26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -1497,19 +1503,19 @@
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E27" s="1">
         <v>45629</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -1520,10 +1526,10 @@
         <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1">
         <v>42025</v>
@@ -1532,7 +1538,7 @@
         <v>859416</v>
       </c>
       <c r="I28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -1543,19 +1549,19 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1">
         <v>43233</v>
       </c>
       <c r="H29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -1566,19 +1572,19 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E30" s="1">
         <v>43078</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -1589,19 +1595,19 @@
         <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E31" s="1">
         <v>42914</v>
       </c>
       <c r="H31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M31">
         <v>1</v>
@@ -1612,10 +1618,10 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E32" s="1">
         <v>42579</v>
@@ -1624,7 +1630,7 @@
         <v>380112</v>
       </c>
       <c r="I32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -1635,10 +1641,10 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E33" s="1">
         <v>44054</v>
@@ -1647,7 +1653,7 @@
         <v>696875</v>
       </c>
       <c r="I33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -1658,19 +1664,19 @@
         <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" s="1">
         <v>42668</v>
       </c>
       <c r="H34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M34">
         <v>1</v>
@@ -1681,10 +1687,10 @@
         <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E35" s="1">
         <v>42875</v>
@@ -1693,7 +1699,7 @@
         <v>193926</v>
       </c>
       <c r="I35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M35">
         <v>1</v>
@@ -1704,19 +1710,19 @@
         <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E36" s="1">
         <v>44359</v>
       </c>
       <c r="H36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -1727,10 +1733,10 @@
         <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E37" s="1">
         <v>42243</v>
@@ -1739,7 +1745,7 @@
         <v>425614</v>
       </c>
       <c r="I37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M37">
         <v>1</v>
@@ -1750,19 +1756,19 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E38" s="1">
         <v>45307</v>
       </c>
       <c r="H38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M38">
         <v>1</v>
@@ -1773,10 +1779,10 @@
         <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E39" s="1">
         <v>44068</v>
@@ -1785,7 +1791,7 @@
         <v>977245</v>
       </c>
       <c r="I39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M39">
         <v>1</v>
@@ -1796,10 +1802,10 @@
         <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E40" s="1">
         <v>44309</v>
@@ -1808,7 +1814,7 @@
         <v>216083</v>
       </c>
       <c r="I40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M40">
         <v>1</v>
@@ -1819,19 +1825,19 @@
         <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E41" s="1">
         <v>43412</v>
       </c>
       <c r="H41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -1842,10 +1848,10 @@
         <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E42" s="1">
         <v>43541</v>
@@ -1854,7 +1860,7 @@
         <v>383030</v>
       </c>
       <c r="I42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M42">
         <v>1</v>
@@ -1865,19 +1871,19 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E43" s="1">
         <v>42989</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M43">
         <v>1</v>
@@ -1888,19 +1894,19 @@
         <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E44" s="1">
         <v>43436</v>
       </c>
       <c r="H44" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M44">
         <v>1</v>
@@ -1911,10 +1917,10 @@
         <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E45" s="1">
         <v>44391</v>
@@ -1923,7 +1929,7 @@
         <v>439917</v>
       </c>
       <c r="I45" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M45">
         <v>1</v>
@@ -1934,10 +1940,10 @@
         <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E46" s="1">
         <v>45176</v>
@@ -1946,7 +1952,7 @@
         <v>748742</v>
       </c>
       <c r="I46" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M46">
         <v>1</v>
@@ -1957,19 +1963,19 @@
         <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E47" s="1">
         <v>42849</v>
       </c>
       <c r="H47" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I47" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -1980,19 +1986,19 @@
         <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E48" s="1">
         <v>43267</v>
       </c>
       <c r="H48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -2003,10 +2009,10 @@
         <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E49" s="1">
         <v>44364</v>
@@ -2015,7 +2021,7 @@
         <v>367015</v>
       </c>
       <c r="I49" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M49">
         <v>1</v>
@@ -2026,19 +2032,19 @@
         <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E50" s="1">
         <v>42936</v>
       </c>
       <c r="H50" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -2049,10 +2055,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E51" s="1">
         <v>43117</v>
@@ -2061,7 +2067,7 @@
         <v>394947</v>
       </c>
       <c r="I51" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M51">
         <v>2</v>
@@ -2072,19 +2078,19 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E52" s="1">
         <v>44027</v>
       </c>
       <c r="H52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M52">
         <v>2</v>
@@ -2095,19 +2101,19 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E53" s="1">
         <v>44835</v>
       </c>
       <c r="H53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I53" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M53">
         <v>2</v>
@@ -2118,10 +2124,10 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E54" s="1">
         <v>43307</v>
@@ -2130,7 +2136,7 @@
         <v>907904</v>
       </c>
       <c r="I54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M54">
         <v>2</v>
@@ -2141,19 +2147,19 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E55" s="1">
         <v>42892</v>
       </c>
       <c r="H55" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M55">
         <v>2</v>
@@ -2164,10 +2170,10 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C56" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E56" s="1">
         <v>44100</v>
@@ -2176,7 +2182,7 @@
         <v>175887</v>
       </c>
       <c r="I56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M56">
         <v>2</v>
@@ -2187,10 +2193,10 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E57" s="1">
         <v>43137</v>
@@ -2199,7 +2205,7 @@
         <v>763857</v>
       </c>
       <c r="I57" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M57">
         <v>2</v>
@@ -2210,10 +2216,10 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E58" s="1">
         <v>43295</v>
@@ -2222,7 +2228,7 @@
         <v>117135</v>
       </c>
       <c r="I58" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M58">
         <v>2</v>
@@ -2233,10 +2239,10 @@
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E59" s="1">
         <v>42189</v>
@@ -2245,7 +2251,7 @@
         <v>168284</v>
       </c>
       <c r="I59" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M59">
         <v>2</v>
@@ -2256,10 +2262,10 @@
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E60" s="1">
         <v>43362</v>
@@ -2268,7 +2274,7 @@
         <v>926512</v>
       </c>
       <c r="I60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M60">
         <v>2</v>
@@ -2279,19 +2285,19 @@
         <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E61" s="1">
         <v>44003</v>
       </c>
       <c r="H61" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I61" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M61">
         <v>2</v>
@@ -2302,10 +2308,10 @@
         <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E62" s="1">
         <v>45474</v>
@@ -2314,7 +2320,7 @@
         <v>886097</v>
       </c>
       <c r="I62" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M62">
         <v>2</v>
@@ -2325,19 +2331,19 @@
         <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E63" s="1">
         <v>43901</v>
       </c>
       <c r="H63" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M63">
         <v>2</v>
@@ -2348,10 +2354,10 @@
         <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E64" s="1">
         <v>43571</v>
@@ -2360,7 +2366,7 @@
         <v>686542</v>
       </c>
       <c r="I64" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M64">
         <v>2</v>
@@ -2371,19 +2377,19 @@
         <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E65" s="1">
         <v>45231</v>
       </c>
       <c r="H65" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M65">
         <v>2</v>
@@ -2394,10 +2400,10 @@
         <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C66" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E66" s="1">
         <v>43948</v>
@@ -2406,7 +2412,7 @@
         <v>262269</v>
       </c>
       <c r="I66" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M66">
         <v>2</v>
@@ -2417,19 +2423,19 @@
         <v>38</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C67" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E67" s="1">
         <v>44920</v>
       </c>
       <c r="H67" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I67" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M67">
         <v>2</v>
@@ -2440,10 +2446,10 @@
         <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E68" s="1">
         <v>44330</v>
@@ -2452,7 +2458,7 @@
         <v>849556</v>
       </c>
       <c r="I68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M68">
         <v>2</v>
@@ -2463,19 +2469,19 @@
         <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C69" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E69" s="1">
         <v>44768</v>
       </c>
       <c r="H69" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I69" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M69">
         <v>2</v>
@@ -2486,19 +2492,19 @@
         <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E70" s="1">
         <v>42160</v>
       </c>
       <c r="H70" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I70" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M70">
         <v>2</v>
@@ -2509,19 +2515,19 @@
         <v>46</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E71" s="1">
         <v>42039</v>
       </c>
       <c r="H71" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I71" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M71">
         <v>2</v>
@@ -2532,19 +2538,19 @@
         <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E72" s="1">
         <v>44942</v>
       </c>
       <c r="H72" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I72" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M72">
         <v>2</v>
@@ -2555,19 +2561,19 @@
         <v>49</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E73" s="1">
         <v>42437</v>
       </c>
       <c r="H73" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I73" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M73">
         <v>2</v>
@@ -2578,10 +2584,10 @@
         <v>52</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E74" s="1">
         <v>43449</v>
@@ -2590,7 +2596,7 @@
         <v>456692</v>
       </c>
       <c r="I74" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M74">
         <v>2</v>
@@ -2601,10 +2607,10 @@
         <v>53</v>
       </c>
       <c r="B75" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E75" s="1">
         <v>42558</v>
@@ -2613,7 +2619,7 @@
         <v>832744</v>
       </c>
       <c r="I75" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M75">
         <v>2</v>
@@ -2624,10 +2630,10 @@
         <v>54</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E76" s="1">
         <v>43885</v>
@@ -2636,7 +2642,7 @@
         <v>519896</v>
       </c>
       <c r="I76" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M76">
         <v>2</v>
@@ -2647,19 +2653,19 @@
         <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C77" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E77" s="1">
         <v>44828</v>
       </c>
       <c r="H77" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I77" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M77">
         <v>2</v>
@@ -2670,10 +2676,10 @@
         <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E78" s="1">
         <v>43459</v>
@@ -2682,7 +2688,7 @@
         <v>123392</v>
       </c>
       <c r="I78" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M78">
         <v>2</v>
@@ -2693,10 +2699,10 @@
         <v>58</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C79" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E79" s="1">
         <v>44021</v>
@@ -2705,7 +2711,7 @@
         <v>395889</v>
       </c>
       <c r="I79" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M79">
         <v>2</v>
@@ -2716,10 +2722,10 @@
         <v>61</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C80" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E80" s="1">
         <v>45571</v>
@@ -2728,7 +2734,7 @@
         <v>144303</v>
       </c>
       <c r="I80" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M80">
         <v>2</v>
@@ -2739,10 +2745,10 @@
         <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E81" s="1">
         <v>43014</v>
@@ -2751,7 +2757,7 @@
         <v>202198</v>
       </c>
       <c r="I81" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M81">
         <v>2</v>
@@ -2762,10 +2768,10 @@
         <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E82" s="1">
         <v>45582</v>
@@ -2774,7 +2780,7 @@
         <v>473939</v>
       </c>
       <c r="I82" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M82">
         <v>2</v>
@@ -2785,19 +2791,19 @@
         <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C83" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E83" s="1">
         <v>44434</v>
       </c>
       <c r="H83" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I83" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M83">
         <v>2</v>
@@ -2808,10 +2814,10 @@
         <v>67</v>
       </c>
       <c r="B84" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E84" s="1">
         <v>45108</v>
@@ -2820,7 +2826,7 @@
         <v>227045</v>
       </c>
       <c r="I84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M84">
         <v>2</v>
@@ -2831,19 +2837,19 @@
         <v>68</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E85" s="1">
         <v>43662</v>
       </c>
       <c r="H85" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I85" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M85">
         <v>2</v>
@@ -2854,19 +2860,19 @@
         <v>69</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E86" s="1">
         <v>44929</v>
       </c>
       <c r="H86" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I86" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M86">
         <v>2</v>
@@ -2877,10 +2883,10 @@
         <v>70</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C87" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E87" s="1">
         <v>44181</v>
@@ -2889,7 +2895,7 @@
         <v>486842</v>
       </c>
       <c r="I87" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M87">
         <v>2</v>
@@ -2900,19 +2906,19 @@
         <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C88" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E88" s="1">
         <v>44290</v>
       </c>
       <c r="H88" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I88" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M88">
         <v>2</v>
@@ -2923,19 +2929,19 @@
         <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E89" s="1">
         <v>42668</v>
       </c>
       <c r="H89" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I89" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M89">
         <v>2</v>
@@ -2946,10 +2952,10 @@
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E90" s="1">
         <v>43103</v>
@@ -2958,7 +2964,7 @@
         <v>872026</v>
       </c>
       <c r="I90" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M90">
         <v>2</v>
@@ -2969,10 +2975,10 @@
         <v>77</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C91" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E91" s="1">
         <v>44685</v>
@@ -2981,7 +2987,7 @@
         <v>747829</v>
       </c>
       <c r="I91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M91">
         <v>2</v>
@@ -2992,10 +2998,10 @@
         <v>81</v>
       </c>
       <c r="B92" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E92" s="1">
         <v>42555</v>
@@ -3004,7 +3010,7 @@
         <v>560542</v>
       </c>
       <c r="I92" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M92">
         <v>2</v>
@@ -3015,10 +3021,10 @@
         <v>87</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C93" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E93" s="1">
         <v>43655</v>
@@ -3027,7 +3033,7 @@
         <v>732577</v>
       </c>
       <c r="I93" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M93">
         <v>2</v>
@@ -3038,19 +3044,19 @@
         <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C94" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E94" s="1">
         <v>42202</v>
       </c>
       <c r="H94" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I94" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M94">
         <v>2</v>
@@ -3061,10 +3067,10 @@
         <v>89</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C95" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E95" s="1">
         <v>42849</v>
@@ -3073,7 +3079,7 @@
         <v>271438</v>
       </c>
       <c r="I95" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M95">
         <v>2</v>
@@ -3084,10 +3090,10 @@
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E96" s="1">
         <v>44156</v>
@@ -3096,7 +3102,7 @@
         <v>362680</v>
       </c>
       <c r="I96" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M96">
         <v>2</v>
@@ -3107,19 +3113,19 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C97" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E97" s="1">
         <v>43319</v>
       </c>
       <c r="H97" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I97" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M97">
         <v>2</v>
@@ -3130,10 +3136,10 @@
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C98" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E98" s="1">
         <v>42743</v>
@@ -3142,7 +3148,7 @@
         <v>499445</v>
       </c>
       <c r="I98" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M98">
         <v>2</v>
@@ -3153,10 +3159,10 @@
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C99" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E99" s="1">
         <v>44938</v>
@@ -3165,7 +3171,7 @@
         <v>355767</v>
       </c>
       <c r="I99" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M99">
         <v>2</v>
@@ -3176,19 +3182,19 @@
         <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C100" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E100" s="1">
         <v>44106</v>
       </c>
       <c r="H100" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I100" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M100">
         <v>2</v>
@@ -3199,10 +3205,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E101" s="1">
         <v>42784</v>
@@ -3211,7 +3217,7 @@
         <v>820971</v>
       </c>
       <c r="I101" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M101">
         <v>2</v>
@@ -3229,9 +3235,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9635F25D-E9A9-4A49-B6C3-EDF6A09A71EB}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:J59"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3245,34 +3251,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3291,10 +3297,10 @@
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3304,7 +3310,7 @@
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(1000,2000)</f>
-        <v>1214</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3324,10 +3330,10 @@
         <v>0.5</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -3337,7 +3343,7 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J59" ca="1" si="0">RANDBETWEEN(1000,2000)</f>
-        <v>1573</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3357,10 +3363,10 @@
         <v>0.5</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -3370,7 +3376,7 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>1243</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3390,10 +3396,10 @@
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -3403,7 +3409,7 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>1341</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3423,10 +3429,10 @@
         <v>0.5</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -3436,7 +3442,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>1107</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3456,10 +3462,10 @@
         <v>0.5</v>
       </c>
       <c r="E7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -3469,7 +3475,7 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>1828</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3489,10 +3495,10 @@
         <v>0.5</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H8">
         <v>7</v>
@@ -3502,7 +3508,7 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>1500</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3522,10 +3528,10 @@
         <v>0.5</v>
       </c>
       <c r="E9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H9">
         <v>8</v>
@@ -3535,7 +3541,7 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>1058</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3555,10 +3561,10 @@
         <v>0.5</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H10">
         <v>8</v>
@@ -3568,7 +3574,7 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>1535</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3588,10 +3594,10 @@
         <v>0.5</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H11">
         <v>8</v>
@@ -3601,7 +3607,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>1924</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3621,10 +3627,10 @@
         <v>0.5</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H12">
         <v>8</v>
@@ -3634,7 +3640,7 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>1323</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3654,10 +3660,10 @@
         <v>0.5</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H13">
         <v>9</v>
@@ -3667,7 +3673,7 @@
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>1816</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3687,10 +3693,10 @@
         <v>0.5</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -3700,7 +3706,7 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>1673</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3720,10 +3726,10 @@
         <v>0.5</v>
       </c>
       <c r="E15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H15">
         <v>13</v>
@@ -3733,7 +3739,7 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>1965</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3753,10 +3759,10 @@
         <v>0.5</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H16">
         <v>13</v>
@@ -3766,7 +3772,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>1070</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3786,10 +3792,10 @@
         <v>0.5</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H17">
         <v>14</v>
@@ -3799,7 +3805,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="0"/>
-        <v>1871</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3819,10 +3825,10 @@
         <v>0.5</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H18">
         <v>14</v>
@@ -3832,7 +3838,7 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="0"/>
-        <v>1726</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3852,10 +3858,10 @@
         <v>0.5</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H19">
         <v>14</v>
@@ -3865,7 +3871,7 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="0"/>
-        <v>1761</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3885,10 +3891,10 @@
         <v>0.5</v>
       </c>
       <c r="E20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H20">
         <v>14</v>
@@ -3898,7 +3904,7 @@
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="0"/>
-        <v>1666</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3918,10 +3924,10 @@
         <v>0.5</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H21">
         <v>15</v>
@@ -3931,7 +3937,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="0"/>
-        <v>1713</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3951,10 +3957,10 @@
         <v>0.5</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H22">
         <v>16</v>
@@ -3964,7 +3970,7 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="0"/>
-        <v>1151</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3984,10 +3990,10 @@
         <v>0.5</v>
       </c>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H23">
         <v>16</v>
@@ -3997,7 +4003,7 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="0"/>
-        <v>1879</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -4017,10 +4023,10 @@
         <v>0.5</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H24">
         <v>17</v>
@@ -4030,7 +4036,7 @@
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="0"/>
-        <v>1632</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -4050,10 +4056,10 @@
         <v>0.5</v>
       </c>
       <c r="E25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H25">
         <v>17</v>
@@ -4063,7 +4069,7 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="0"/>
-        <v>1053</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -4083,10 +4089,10 @@
         <v>0.5</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H26">
         <v>18</v>
@@ -4096,7 +4102,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="0"/>
-        <v>1450</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -4116,10 +4122,10 @@
         <v>0.5</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H27">
         <v>19</v>
@@ -4129,7 +4135,7 @@
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="0"/>
-        <v>1014</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -4149,10 +4155,10 @@
         <v>0.5</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H28">
         <v>21</v>
@@ -4162,7 +4168,7 @@
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="0"/>
-        <v>1812</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -4182,10 +4188,10 @@
         <v>0.5</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H29">
         <v>21</v>
@@ -4195,7 +4201,7 @@
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="0"/>
-        <v>1647</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -4215,10 +4221,10 @@
         <v>0.5</v>
       </c>
       <c r="E30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H30">
         <v>22</v>
@@ -4228,7 +4234,7 @@
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="0"/>
-        <v>1064</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -4248,10 +4254,10 @@
         <v>0.5</v>
       </c>
       <c r="E31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H31">
         <v>22</v>
@@ -4261,7 +4267,7 @@
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="0"/>
-        <v>1545</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -4281,10 +4287,10 @@
         <v>0.5</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H32">
         <v>23</v>
@@ -4294,7 +4300,7 @@
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="0"/>
-        <v>1944</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -4314,10 +4320,10 @@
         <v>0.5</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H33">
         <v>24</v>
@@ -4327,7 +4333,7 @@
       </c>
       <c r="J33">
         <f t="shared" ca="1" si="0"/>
-        <v>1235</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -4347,10 +4353,10 @@
         <v>0.5</v>
       </c>
       <c r="E34" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F34" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H34">
         <v>24</v>
@@ -4360,7 +4366,7 @@
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="0"/>
-        <v>1022</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -4380,10 +4386,10 @@
         <v>0.5</v>
       </c>
       <c r="E35" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F35" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H35">
         <v>24</v>
@@ -4393,7 +4399,7 @@
       </c>
       <c r="J35">
         <f t="shared" ca="1" si="0"/>
-        <v>1272</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -4413,10 +4419,10 @@
         <v>0.5</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F36" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H36">
         <v>26</v>
@@ -4426,7 +4432,7 @@
       </c>
       <c r="J36">
         <f t="shared" ca="1" si="0"/>
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -4446,10 +4452,10 @@
         <v>0.5</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F37" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H37">
         <v>27</v>
@@ -4459,7 +4465,7 @@
       </c>
       <c r="J37">
         <f t="shared" ca="1" si="0"/>
-        <v>1383</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4479,10 +4485,10 @@
         <v>0.5</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H38">
         <v>29</v>
@@ -4492,7 +4498,7 @@
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="0"/>
-        <v>1348</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -4512,10 +4518,10 @@
         <v>0.5</v>
       </c>
       <c r="E39" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F39" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H39">
         <v>30</v>
@@ -4525,7 +4531,7 @@
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="0"/>
-        <v>1730</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -4545,10 +4551,10 @@
         <v>0.5</v>
       </c>
       <c r="E40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H40">
         <v>30</v>
@@ -4558,7 +4564,7 @@
       </c>
       <c r="J40">
         <f t="shared" ca="1" si="0"/>
-        <v>1288</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -4578,10 +4584,10 @@
         <v>0.5</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H41">
         <v>30</v>
@@ -4591,7 +4597,7 @@
       </c>
       <c r="J41">
         <f t="shared" ca="1" si="0"/>
-        <v>1991</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -4611,10 +4617,10 @@
         <v>0.5</v>
       </c>
       <c r="E42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H42">
         <v>32</v>
@@ -4624,7 +4630,7 @@
       </c>
       <c r="J42">
         <f t="shared" ca="1" si="0"/>
-        <v>1664</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -4644,10 +4650,10 @@
         <v>0.5</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H43">
         <v>33</v>
@@ -4657,7 +4663,7 @@
       </c>
       <c r="J43">
         <f t="shared" ca="1" si="0"/>
-        <v>1645</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -4677,10 +4683,10 @@
         <v>0.5</v>
       </c>
       <c r="E44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H44">
         <v>33</v>
@@ -4690,7 +4696,7 @@
       </c>
       <c r="J44">
         <f t="shared" ca="1" si="0"/>
-        <v>1784</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -4710,10 +4716,10 @@
         <v>0.5</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H45">
         <v>34</v>
@@ -4723,7 +4729,7 @@
       </c>
       <c r="J45">
         <f t="shared" ca="1" si="0"/>
-        <v>1886</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -4743,10 +4749,10 @@
         <v>0.5</v>
       </c>
       <c r="E46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H46">
         <v>34</v>
@@ -4756,7 +4762,7 @@
       </c>
       <c r="J46">
         <f t="shared" ca="1" si="0"/>
-        <v>1802</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -4776,10 +4782,10 @@
         <v>0.5</v>
       </c>
       <c r="E47" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H47">
         <v>35</v>
@@ -4789,7 +4795,7 @@
       </c>
       <c r="J47">
         <f t="shared" ca="1" si="0"/>
-        <v>1042</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -4809,10 +4815,10 @@
         <v>0.5</v>
       </c>
       <c r="E48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H48">
         <v>39</v>
@@ -4822,7 +4828,7 @@
       </c>
       <c r="J48">
         <f t="shared" ca="1" si="0"/>
-        <v>1031</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -4842,10 +4848,10 @@
         <v>0.5</v>
       </c>
       <c r="E49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H49">
         <v>43</v>
@@ -4855,7 +4861,7 @@
       </c>
       <c r="J49">
         <f t="shared" ca="1" si="0"/>
-        <v>1891</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -4875,10 +4881,10 @@
         <v>0.5</v>
       </c>
       <c r="E50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H50">
         <v>48</v>
@@ -4888,7 +4894,7 @@
       </c>
       <c r="J50">
         <f t="shared" ca="1" si="0"/>
-        <v>1558</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -4908,10 +4914,10 @@
         <v>0.5</v>
       </c>
       <c r="E51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H51">
         <v>50</v>
@@ -4921,7 +4927,7 @@
       </c>
       <c r="J51">
         <f t="shared" ca="1" si="0"/>
-        <v>1070</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -4938,22 +4944,22 @@
         <v>0.5</v>
       </c>
       <c r="E52" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F52" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G52" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J52">
         <f t="shared" ca="1" si="0"/>
-        <v>1422</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -4965,17 +4971,17 @@
         <v>0.5</v>
       </c>
       <c r="E53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J53">
         <f t="shared" ca="1" si="0"/>
-        <v>1834</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -4989,22 +4995,22 @@
         <v>0.5</v>
       </c>
       <c r="E54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J54">
         <f t="shared" ca="1" si="0"/>
-        <v>1652</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C55" s="1">
         <v>44505</v>
@@ -5013,22 +5019,22 @@
         <v>0.5</v>
       </c>
       <c r="E55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J55">
         <f t="shared" ca="1" si="0"/>
-        <v>1121</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5037,22 +5043,22 @@
         <v>0.5</v>
       </c>
       <c r="E56" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F56" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G56" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J56">
         <f t="shared" ca="1" si="0"/>
-        <v>1231</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5061,22 +5067,22 @@
         <v>44321</v>
       </c>
       <c r="E57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G57" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J57">
         <f t="shared" ca="1" si="0"/>
-        <v>1869</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -5088,22 +5094,22 @@
         <v>0.5</v>
       </c>
       <c r="E58" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F58" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G58" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J58">
         <f t="shared" ca="1" si="0"/>
-        <v>1520</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B59">
         <v>13</v>
@@ -5115,11 +5121,11 @@
         <v>0.5</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J59">
         <f t="shared" ca="1" si="0"/>
-        <v>1128</v>
+        <v>1931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>